<commit_message>
feat Upd excel  backup Crossell y Renovacion y Pagos
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/CrossellRenovacion.xlsx
+++ b/src/test/resources/dataDriven/CrossellRenovacion.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/candyespinzabaez/Documents/Android/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC190DF-D2CB-FB4B-B551-F78703F4358B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCA5723-F9E4-C040-91E3-5B9BDFE35193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="9520" windowWidth="26000" windowHeight="10880" activeTab="4" xr2:uid="{897FEA26-AEC5-9349-951A-1C74BA5F166B}"/>
+    <workbookView xWindow="1020" yWindow="6620" windowWidth="26000" windowHeight="10880" xr2:uid="{897FEA26-AEC5-9349-951A-1C74BA5F166B}"/>
   </bookViews>
   <sheets>
     <sheet name="Indice" sheetId="16" r:id="rId1"/>
@@ -18,10 +18,12 @@
     <sheet name="PerfiladorVehicular" sheetId="23" r:id="rId3"/>
     <sheet name="TiempoInactividadCrossellyRenov" sheetId="24" r:id="rId4"/>
     <sheet name="CompraSOATDigital" sheetId="25" r:id="rId5"/>
+    <sheet name="CompraSOATVial" sheetId="26" r:id="rId6"/>
+    <sheet name="CompraSOATPlus" sheetId="27" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
   <si>
     <t>usar</t>
   </si>
@@ -91,9 +93,6 @@
     <t>@CompraSOATDigital</t>
   </si>
   <si>
-    <t>Plan SOAT(DIGITAL)</t>
-  </si>
-  <si>
     <t>Rimac2021</t>
   </si>
   <si>
@@ -131,13 +130,39 @@
   </si>
   <si>
     <t>AXT435</t>
+  </si>
+  <si>
+    <t>07525151</t>
+  </si>
+  <si>
+    <t>AXT243</t>
+  </si>
+  <si>
+    <t>AXT485</t>
+  </si>
+  <si>
+    <t>07546167</t>
+  </si>
+  <si>
+    <t>@CompraSOATVial</t>
+  </si>
+  <si>
+    <t>@CompraSOATPlus</t>
+  </si>
+  <si>
+    <t>Compra seguro SOAT &lt;placa&gt;  - Plan Vial</t>
+  </si>
+  <si>
+    <t>Compra seguro SOAT &lt;placa&gt;  - Plan SOAT(DIGITAL)</t>
+  </si>
+  <si>
+    <t>Compra seguro SOAT &lt;placa&gt; - Plan Soat Plus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -224,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,14 +276,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -581,18 +609,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13795FAB-EE90-174B-9401-A5700886F2BE}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.6640625"/>
-    <col min="2" max="2" customWidth="true" width="37.6640625"/>
-    <col min="3" max="3" customWidth="true" width="77.1640625"/>
-    <col min="4" max="4" customWidth="true" style="3" width="8.1640625"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="77.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -610,7 +638,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -624,7 +652,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
@@ -636,7 +664,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
@@ -648,26 +676,52 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A2:A7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" location="PerfiladorSalud!A1" display="Aqui" xr:uid="{DA0C6991-452B-8540-A26F-849EE2F6F725}"/>
     <hyperlink ref="D3" location="PerfiladorVehicular!A1" display="Aqui" xr:uid="{ACBA14B9-AF0B-F64B-A18A-105A6AAF0225}"/>
     <hyperlink ref="D4" location="TiempoInactividadCrossellyRenov!A1" display="Aqui" xr:uid="{C85FD113-192C-3347-A277-077FA647CD53}"/>
     <hyperlink ref="D5" location="CompraSOATDigital!A1" display="Aqui" xr:uid="{6E1131A7-587E-6347-95FB-4C44D5D5220A}"/>
+    <hyperlink ref="D6:D7" location="CompraSOATVial!A1" display="Aqui" xr:uid="{737EF2A3-55B5-624B-BCA5-1876C18B631D}"/>
+    <hyperlink ref="D7" location="CompraSOATPlus!A1" display="Aqui" xr:uid="{33A0B116-AC8E-494A-AF07-FBC34ABA8D01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -703,10 +757,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -747,13 +801,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +823,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -786,16 +840,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -806,22 +860,22 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="13" t="s">
         <v>25</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -833,11 +887,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDE23C9-1EB8-1F45-A88F-E4F4E4209918}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -854,16 +910,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -874,22 +930,160 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71F9821-44F0-654E-ABE2-AC8E0AAEC5E2}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE958D98-3918-284A-8CD0-726FF9E1A1D5}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat ups escenario venta nueva
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/CrossellRenovacion.xlsx
+++ b/src/test/resources/dataDriven/CrossellRenovacion.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/candyespinzabaez/Documents/Android/"/>
     </mc:Choice>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -163,6 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -617,10 +618,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="3" max="3" width="77.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.6640625"/>
+    <col min="2" max="2" customWidth="true" width="37.6640625"/>
+    <col min="3" max="3" customWidth="true" width="77.1640625"/>
+    <col min="4" max="4" customWidth="true" style="3" width="8.1640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -823,7 +824,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -893,7 +894,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -963,7 +964,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1031,7 +1032,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>